<commit_message>
corrections to Data Model and Scripts for upload
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/Archive.xlsx
+++ b/data/Spreadsheet_Data/Archive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44324461-0D06-7440-831B-5111F26EB515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABC225C-E779-B24F-B285-5A5E475F1455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18220" yWindow="4180" windowWidth="27700" windowHeight="16940" xr2:uid="{7AF20345-843F-AC45-893A-6EE522003F38}"/>
   </bookViews>
@@ -58,7 +58,7 @@
     <t>Spreadsheet_Data.zip</t>
   </si>
   <si>
-    <t>data/Multimedia_Data/Dungeon/</t>
+    <t>data/Multimedia_Data/Archive/</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Character and Book Chapter
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/Archive.xlsx
+++ b/data/Spreadsheet_Data/Archive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABC225C-E779-B24F-B285-5A5E475F1455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F1B0F9-41B2-1740-926A-8F875C2AEA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18220" yWindow="4180" windowWidth="27700" windowHeight="16940" xr2:uid="{7AF20345-843F-AC45-893A-6EE522003F38}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>D_001</t>
-  </si>
-  <si>
     <t>File Name</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>data/Multimedia_Data/Archive/</t>
+  </si>
+  <si>
+    <t>AR_001</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -446,24 +446,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>